<commit_message>
dev: update example sheet
</commit_message>
<xml_diff>
--- a/test/data/bacnet-ip-mode-test-sheet.xlsx
+++ b/test/data/bacnet-ip-mode-test-sheet.xlsx
@@ -1233,7 +1233,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="4"/>
@@ -1268,7 +1268,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -1285,7 +1285,7 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -1302,7 +1302,7 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
dev: update test bacnet sheet
</commit_message>
<xml_diff>
--- a/test/data/bacnet-ip-mode-test-sheet.xlsx
+++ b/test/data/bacnet-ip-mode-test-sheet.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="40">
   <si>
     <t>tag</t>
   </si>
@@ -44,16 +44,109 @@
     <t>objectId</t>
   </si>
   <si>
-    <t>temp</t>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>温度</t>
   </si>
   <si>
     <t>AI</t>
   </si>
   <si>
-    <t>humi</t>
-  </si>
-  <si>
-    <t>gas</t>
+    <t>Humidity</t>
+  </si>
+  <si>
+    <t>湿度</t>
+  </si>
+  <si>
+    <t>ConOxygen</t>
+  </si>
+  <si>
+    <t>氧气浓度</t>
+  </si>
+  <si>
+    <t>Conductive</t>
+  </si>
+  <si>
+    <t>电导率</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>PH值</t>
+  </si>
+  <si>
+    <t>DisOxygen</t>
+  </si>
+  <si>
+    <t>溶解氧</t>
+  </si>
+  <si>
+    <t>ConChlorophyll</t>
+  </si>
+  <si>
+    <t>叶绿素</t>
+  </si>
+  <si>
+    <t>Phycocyanin</t>
+  </si>
+  <si>
+    <t>藻蓝素</t>
+  </si>
+  <si>
+    <t>Light</t>
+  </si>
+  <si>
+    <t>光透度</t>
+  </si>
+  <si>
+    <t>Wave</t>
+  </si>
+  <si>
+    <t>波动值</t>
+  </si>
+  <si>
+    <t>Density</t>
+  </si>
+  <si>
+    <t>密度</t>
+  </si>
+  <si>
+    <t>Vibration</t>
+  </si>
+  <si>
+    <t>振动</t>
+  </si>
+  <si>
+    <t>AirPressure</t>
+  </si>
+  <si>
+    <t>气压</t>
+  </si>
+  <si>
+    <t>WindSpeed</t>
+  </si>
+  <si>
+    <t>风速</t>
+  </si>
+  <si>
+    <t>WindDirection</t>
+  </si>
+  <si>
+    <t>风向</t>
+  </si>
+  <si>
+    <t>ConFormaldehyde</t>
+  </si>
+  <si>
+    <t>甲醛浓度</t>
+  </si>
+  <si>
+    <t>MicrobialCount</t>
+  </si>
+  <si>
+    <t>微生物数量</t>
   </si>
 </sst>
 </file>
@@ -227,7 +320,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,6 +330,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -574,7 +679,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -598,16 +703,16 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -616,93 +721,99 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1230,14 +1341,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="10.875" customWidth="1"/>
     <col min="3" max="3" width="17.875" customWidth="1"/>
     <col min="4" max="4" width="12.875" customWidth="1"/>
     <col min="5" max="5" width="10.375" customWidth="1"/>
@@ -1261,54 +1374,581 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2">
         <v>5</v>
       </c>
-      <c r="C2">
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="2">
         <v>6</v>
       </c>
-      <c r="E2">
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
+    <row r="20" spans="1:5">
+      <c r="A20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="3">
         <v>6</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="3">
+        <v>2</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="3">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4">
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="3">
         <v>2</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="3">
+        <v>2</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" s="3">
+        <v>2</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="3">
+        <v>2</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="3">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>